<commit_message>
change instructions to reflect excel better. add advanced main analysis, which allows parameter changes.
</commit_message>
<xml_diff>
--- a/excel_templates/analysis_info.xlsx
+++ b/excel_templates/analysis_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfrahm/Code/ALE/new_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfrahm/Code/ALE/pyALE/excel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE32DB0-2EF7-844D-B6D0-38420B3CE1A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E1B35E-0F7F-9348-BC42-B58E75FCD8B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28000" yWindow="15260" windowWidth="27920" windowHeight="16300" xr2:uid="{0A56B9C8-76CD-1B4B-B14E-A677B9DAC1B9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>M</t>
   </si>
@@ -36,25 +36,37 @@
     <t>P17</t>
   </si>
   <si>
-    <t>B17</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>+Other</t>
-  </si>
-  <si>
-    <t>+I&gt;C</t>
-  </si>
-  <si>
-    <t>Cwclassic</t>
-  </si>
-  <si>
-    <t>+CW</t>
-  </si>
-  <si>
-    <t>+Colorword</t>
+    <t>Title1</t>
+  </si>
+  <si>
+    <t>+Tag1</t>
+  </si>
+  <si>
+    <t>+Tag2</t>
+  </si>
+  <si>
+    <t>Title2</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Title3</t>
+  </si>
+  <si>
+    <t>+ALL</t>
+  </si>
+  <si>
+    <t>Title4</t>
+  </si>
+  <si>
+    <t>-Tag2</t>
+  </si>
+  <si>
+    <t>$mask.nii</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -416,7 +428,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,13 +443,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -445,27 +457,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -473,41 +485,38 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add cmd_pipeline. change coding of columnes in exp_info read in. add parameter settings to nb_pipeline.
</commit_message>
<xml_diff>
--- a/excel_templates/analysis_info.xlsx
+++ b/excel_templates/analysis_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfrahm/Code/ALE/pyALE/excel_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfrahm/Code/ALE/pyALE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E1B35E-0F7F-9348-BC42-B58E75FCD8B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1F142B-551D-C24F-8FCC-AB60DB51CE68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28000" yWindow="15260" windowWidth="27920" windowHeight="16300" xr2:uid="{0A56B9C8-76CD-1B4B-B14E-A677B9DAC1B9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>M</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>+Other</t>
+  </si>
+  <si>
+    <t>+I&gt;C</t>
   </si>
 </sst>
 </file>
@@ -428,7 +437,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,13 +452,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>